<commit_message>
updated excel error handling/fixed timestamp
</commit_message>
<xml_diff>
--- a/UpdatedFiles/CSProvisioning.xlsx
+++ b/UpdatedFiles/CSProvisioning.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3859" uniqueCount="1835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="1835">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -7093,6 +7093,9 @@
       <c r="G42" t="s">
         <v>1039</v>
       </c>
+      <c r="I42" t="s">
+        <v>1081</v>
+      </c>
       <c r="J42" t="s">
         <v>1346</v>
       </c>
@@ -7119,6 +7122,9 @@
       <c r="G43" t="s">
         <v>1042</v>
       </c>
+      <c r="I43" t="s">
+        <v>1081</v>
+      </c>
       <c r="J43" t="s">
         <v>1347</v>
       </c>
@@ -7348,6 +7354,9 @@
       <c r="G51" t="s">
         <v>1039</v>
       </c>
+      <c r="I51" t="s">
+        <v>1086</v>
+      </c>
       <c r="J51" t="s">
         <v>1346</v>
       </c>
@@ -7516,6 +7525,9 @@
       <c r="G57" t="s">
         <v>1036</v>
       </c>
+      <c r="I57" t="s">
+        <v>1088</v>
+      </c>
       <c r="J57" t="s">
         <v>1347</v>
       </c>
@@ -7542,6 +7554,9 @@
       <c r="G58" t="s">
         <v>1040</v>
       </c>
+      <c r="I58" t="s">
+        <v>1088</v>
+      </c>
       <c r="J58" t="s">
         <v>1346</v>
       </c>
@@ -8925,6 +8940,9 @@
       <c r="G106" t="s">
         <v>1043</v>
       </c>
+      <c r="I106" t="s">
+        <v>1127</v>
+      </c>
       <c r="J106" t="s">
         <v>1348</v>
       </c>
@@ -8951,6 +8969,9 @@
       <c r="G107" t="s">
         <v>1039</v>
       </c>
+      <c r="I107" t="s">
+        <v>1127</v>
+      </c>
       <c r="J107" t="s">
         <v>1348</v>
       </c>
@@ -9093,6 +9114,9 @@
       <c r="G112" t="s">
         <v>1039</v>
       </c>
+      <c r="I112" t="s">
+        <v>1130</v>
+      </c>
       <c r="J112" t="s">
         <v>1348</v>
       </c>
@@ -9322,6 +9346,9 @@
       <c r="G120" t="s">
         <v>1045</v>
       </c>
+      <c r="I120" t="s">
+        <v>1134</v>
+      </c>
       <c r="J120" t="s">
         <v>1347</v>
       </c>
@@ -9348,6 +9375,9 @@
       <c r="G121" t="s">
         <v>1039</v>
       </c>
+      <c r="I121" t="s">
+        <v>1134</v>
+      </c>
       <c r="J121" t="s">
         <v>1348</v>
       </c>
@@ -9490,6 +9520,9 @@
       <c r="G126" t="s">
         <v>1039</v>
       </c>
+      <c r="I126" t="s">
+        <v>1136</v>
+      </c>
       <c r="J126" t="s">
         <v>1348</v>
       </c>
@@ -9516,6 +9549,9 @@
       <c r="G127" t="s">
         <v>1041</v>
       </c>
+      <c r="I127" t="s">
+        <v>1136</v>
+      </c>
       <c r="J127" t="s">
         <v>1348</v>
       </c>
@@ -9710,6 +9746,9 @@
       <c r="G134" t="s">
         <v>1039</v>
       </c>
+      <c r="I134" t="s">
+        <v>1139</v>
+      </c>
       <c r="J134" t="s">
         <v>1348</v>
       </c>
@@ -9736,6 +9775,9 @@
       <c r="G135" t="s">
         <v>1039</v>
       </c>
+      <c r="I135" t="s">
+        <v>1139</v>
+      </c>
       <c r="J135" t="s">
         <v>1348</v>
       </c>
@@ -10023,6 +10065,9 @@
       <c r="G145" t="s">
         <v>1039</v>
       </c>
+      <c r="I145" t="s">
+        <v>1145</v>
+      </c>
       <c r="J145" t="s">
         <v>1349</v>
       </c>
@@ -10049,6 +10094,9 @@
       <c r="G146" t="s">
         <v>1036</v>
       </c>
+      <c r="I146" t="s">
+        <v>1145</v>
+      </c>
       <c r="J146" t="s">
         <v>1346</v>
       </c>
@@ -10356,6 +10404,9 @@
       <c r="G157" t="s">
         <v>1036</v>
       </c>
+      <c r="I157" t="s">
+        <v>1150</v>
+      </c>
       <c r="J157" t="s">
         <v>1347</v>
       </c>
@@ -10382,6 +10433,9 @@
       <c r="G158" t="s">
         <v>1036</v>
       </c>
+      <c r="I158" t="s">
+        <v>1150</v>
+      </c>
       <c r="J158" t="s">
         <v>1347</v>
       </c>
@@ -10466,6 +10520,9 @@
       <c r="G161" t="s">
         <v>1036</v>
       </c>
+      <c r="I161" t="s">
+        <v>1151</v>
+      </c>
       <c r="J161" t="s">
         <v>1345</v>
       </c>
@@ -10492,6 +10549,9 @@
       <c r="G162" t="s">
         <v>1039</v>
       </c>
+      <c r="I162" t="s">
+        <v>1151</v>
+      </c>
       <c r="J162" t="s">
         <v>1348</v>
       </c>
@@ -10741,6 +10801,9 @@
       <c r="G171" t="s">
         <v>1036</v>
       </c>
+      <c r="I171" t="s">
+        <v>1155</v>
+      </c>
       <c r="J171" t="s">
         <v>1347</v>
       </c>
@@ -10767,6 +10830,9 @@
       <c r="G172" t="s">
         <v>1042</v>
       </c>
+      <c r="I172" t="s">
+        <v>1155</v>
+      </c>
       <c r="J172" t="s">
         <v>1347</v>
       </c>
@@ -10851,6 +10917,9 @@
       <c r="G175" t="s">
         <v>1036</v>
       </c>
+      <c r="I175" t="s">
+        <v>1156</v>
+      </c>
       <c r="J175" t="s">
         <v>1346</v>
       </c>
@@ -10935,6 +11004,9 @@
       <c r="G178" t="s">
         <v>1038</v>
       </c>
+      <c r="I178" t="s">
+        <v>1157</v>
+      </c>
       <c r="J178" t="s">
         <v>1346</v>
       </c>
@@ -11048,6 +11120,9 @@
       <c r="G182" t="s">
         <v>1036</v>
       </c>
+      <c r="I182" t="s">
+        <v>1159</v>
+      </c>
       <c r="J182" t="s">
         <v>1346</v>
       </c>
@@ -11496,6 +11571,9 @@
       <c r="G199" t="s">
         <v>1036</v>
       </c>
+      <c r="I199" t="s">
+        <v>1160</v>
+      </c>
       <c r="J199" t="s">
         <v>1347</v>
       </c>
@@ -11522,6 +11600,9 @@
       <c r="G200" t="s">
         <v>1042</v>
       </c>
+      <c r="I200" t="s">
+        <v>1160</v>
+      </c>
       <c r="J200" t="s">
         <v>1347</v>
       </c>
@@ -11664,6 +11745,9 @@
       <c r="G205" t="s">
         <v>1036</v>
       </c>
+      <c r="I205" t="s">
+        <v>1163</v>
+      </c>
       <c r="J205" t="s">
         <v>1347</v>
       </c>
@@ -11922,6 +12006,9 @@
       <c r="G214" t="s">
         <v>1040</v>
       </c>
+      <c r="I214" t="s">
+        <v>1168</v>
+      </c>
       <c r="J214" t="s">
         <v>1348</v>
       </c>
@@ -11948,6 +12035,9 @@
       <c r="G215" t="s">
         <v>1036</v>
       </c>
+      <c r="I215" t="s">
+        <v>1168</v>
+      </c>
       <c r="J215" t="s">
         <v>1346</v>
       </c>
@@ -12090,6 +12180,9 @@
       <c r="G220" t="s">
         <v>1040</v>
       </c>
+      <c r="I220" t="s">
+        <v>1171</v>
+      </c>
       <c r="J220" t="s">
         <v>1346</v>
       </c>
@@ -12232,6 +12325,9 @@
       <c r="G225" t="s">
         <v>1036</v>
       </c>
+      <c r="I225" t="s">
+        <v>1174</v>
+      </c>
       <c r="J225" t="s">
         <v>1346</v>
       </c>
@@ -12519,6 +12615,9 @@
       <c r="G235" t="s">
         <v>1039</v>
       </c>
+      <c r="I235" t="s">
+        <v>1180</v>
+      </c>
       <c r="J235" t="s">
         <v>1346</v>
       </c>
@@ -12603,6 +12702,9 @@
       <c r="G238" t="s">
         <v>1039</v>
       </c>
+      <c r="I238" t="s">
+        <v>1181</v>
+      </c>
       <c r="J238" t="s">
         <v>1348</v>
       </c>
@@ -12629,6 +12731,9 @@
       <c r="G239" t="s">
         <v>1039</v>
       </c>
+      <c r="I239" t="s">
+        <v>1181</v>
+      </c>
       <c r="J239" t="s">
         <v>1348</v>
       </c>
@@ -12713,6 +12818,9 @@
       <c r="G242" t="s">
         <v>1039</v>
       </c>
+      <c r="I242" t="s">
+        <v>1182</v>
+      </c>
       <c r="J242" t="s">
         <v>1348</v>
       </c>
@@ -12884,6 +12992,9 @@
       <c r="G248" t="s">
         <v>1046</v>
       </c>
+      <c r="I248" t="s">
+        <v>1185</v>
+      </c>
       <c r="J248" t="s">
         <v>1348</v>
       </c>
@@ -13606,6 +13717,9 @@
       <c r="G273" t="s">
         <v>1036</v>
       </c>
+      <c r="I273" t="s">
+        <v>1208</v>
+      </c>
       <c r="J273" t="s">
         <v>1347</v>
       </c>
@@ -13806,6 +13920,9 @@
       <c r="G280" t="s">
         <v>1039</v>
       </c>
+      <c r="I280" t="s">
+        <v>1212</v>
+      </c>
       <c r="J280" t="s">
         <v>1346</v>
       </c>
@@ -14006,6 +14123,9 @@
       <c r="G287" t="s">
         <v>1039</v>
       </c>
+      <c r="I287" t="s">
+        <v>1216</v>
+      </c>
       <c r="J287" t="s">
         <v>1348</v>
       </c>
@@ -14438,6 +14558,9 @@
       <c r="G302" t="s">
         <v>1041</v>
       </c>
+      <c r="I302" t="s">
+        <v>1226</v>
+      </c>
       <c r="J302" t="s">
         <v>1346</v>
       </c>
@@ -14464,6 +14587,9 @@
       <c r="G303" t="s">
         <v>1042</v>
       </c>
+      <c r="I303" t="s">
+        <v>1226</v>
+      </c>
       <c r="J303" t="s">
         <v>1347</v>
       </c>
@@ -15563,6 +15689,9 @@
       <c r="G341" t="s">
         <v>1045</v>
       </c>
+      <c r="I341" t="s">
+        <v>1252</v>
+      </c>
       <c r="J341" t="s">
         <v>1346</v>
       </c>
@@ -15589,6 +15718,9 @@
       <c r="G342" t="s">
         <v>1039</v>
       </c>
+      <c r="I342" t="s">
+        <v>1252</v>
+      </c>
       <c r="J342" t="s">
         <v>1348</v>
       </c>
@@ -16050,6 +16182,9 @@
       <c r="G358" t="s">
         <v>1036</v>
       </c>
+      <c r="I358" t="s">
+        <v>1263</v>
+      </c>
       <c r="J358" t="s">
         <v>1347</v>
       </c>
@@ -16076,6 +16211,9 @@
       <c r="G359" t="s">
         <v>1044</v>
       </c>
+      <c r="I359" t="s">
+        <v>1263</v>
+      </c>
       <c r="J359" t="s">
         <v>1346</v>
       </c>
@@ -17140,6 +17278,9 @@
       <c r="G396" t="s">
         <v>1039</v>
       </c>
+      <c r="I396" t="s">
+        <v>1293</v>
+      </c>
       <c r="J396" t="s">
         <v>1348</v>
       </c>
@@ -17166,6 +17307,9 @@
       <c r="G397" t="s">
         <v>1039</v>
       </c>
+      <c r="I397" t="s">
+        <v>1293</v>
+      </c>
       <c r="J397" t="s">
         <v>1348</v>
       </c>
@@ -17424,6 +17568,9 @@
       <c r="G406" t="s">
         <v>1042</v>
       </c>
+      <c r="I406" t="s">
+        <v>1297</v>
+      </c>
       <c r="J406" t="s">
         <v>1347</v>
       </c>
@@ -17450,6 +17597,9 @@
       <c r="G407" t="s">
         <v>1039</v>
       </c>
+      <c r="I407" t="s">
+        <v>1297</v>
+      </c>
       <c r="J407" t="s">
         <v>1346</v>
       </c>
@@ -18346,6 +18496,9 @@
       <c r="G438" t="s">
         <v>1036</v>
       </c>
+      <c r="I438" t="s">
+        <v>1322</v>
+      </c>
       <c r="J438" t="s">
         <v>1347</v>
       </c>
@@ -19027,8 +19180,23 @@
       <c r="B462" t="s">
         <v>471</v>
       </c>
+      <c r="D462" t="s">
+        <v>523</v>
+      </c>
+      <c r="E462" t="s">
+        <v>523</v>
+      </c>
       <c r="F462" t="s">
         <v>986</v>
+      </c>
+      <c r="G462" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I462" t="s">
+        <v>1339</v>
+      </c>
+      <c r="J462" t="s">
+        <v>1346</v>
       </c>
       <c r="K462" t="s">
         <v>986</v>
@@ -19153,8 +19321,20 @@
       <c r="B468" t="s">
         <v>477</v>
       </c>
+      <c r="D468" t="s">
+        <v>523</v>
+      </c>
+      <c r="E468" t="s">
+        <v>523</v>
+      </c>
       <c r="F468" t="s">
         <v>992</v>
+      </c>
+      <c r="I468" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J468" t="s">
+        <v>1346</v>
       </c>
       <c r="K468" t="s">
         <v>992</v>
@@ -19167,8 +19347,20 @@
       <c r="B469" t="s">
         <v>478</v>
       </c>
+      <c r="D469" t="s">
+        <v>523</v>
+      </c>
+      <c r="E469" t="s">
+        <v>523</v>
+      </c>
       <c r="F469" t="s">
         <v>993</v>
+      </c>
+      <c r="I469" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J469" t="s">
+        <v>1346</v>
       </c>
       <c r="K469" t="s">
         <v>993</v>
@@ -19289,8 +19481,17 @@
       <c r="B476" t="s">
         <v>484</v>
       </c>
+      <c r="D476" t="s">
+        <v>525</v>
+      </c>
+      <c r="E476" t="s">
+        <v>525</v>
+      </c>
       <c r="F476" t="s">
         <v>999</v>
+      </c>
+      <c r="J476" t="s">
+        <v>1346</v>
       </c>
       <c r="K476" t="s">
         <v>999</v>
@@ -19303,8 +19504,17 @@
       <c r="B477" t="s">
         <v>485</v>
       </c>
+      <c r="D477" t="s">
+        <v>525</v>
+      </c>
+      <c r="E477" t="s">
+        <v>525</v>
+      </c>
       <c r="F477" t="s">
         <v>1000</v>
+      </c>
+      <c r="J477" t="s">
+        <v>1346</v>
       </c>
       <c r="K477" t="s">
         <v>1000</v>
@@ -19391,8 +19601,23 @@
       <c r="B482" t="s">
         <v>490</v>
       </c>
+      <c r="D482" t="s">
+        <v>523</v>
+      </c>
+      <c r="E482" t="s">
+        <v>523</v>
+      </c>
       <c r="F482" t="s">
         <v>1005</v>
+      </c>
+      <c r="G482" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I482" t="s">
+        <v>1341</v>
+      </c>
+      <c r="J482" t="s">
+        <v>1346</v>
       </c>
       <c r="K482" t="s">
         <v>1005</v>
@@ -19405,8 +19630,23 @@
       <c r="B483" t="s">
         <v>491</v>
       </c>
+      <c r="D483" t="s">
+        <v>523</v>
+      </c>
+      <c r="E483" t="s">
+        <v>523</v>
+      </c>
       <c r="F483" t="s">
         <v>1006</v>
+      </c>
+      <c r="G483" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I483" t="s">
+        <v>1341</v>
+      </c>
+      <c r="J483" t="s">
+        <v>1346</v>
       </c>
       <c r="K483" t="s">
         <v>1006</v>
@@ -19491,8 +19731,23 @@
       <c r="B487" t="s">
         <v>495</v>
       </c>
+      <c r="D487" t="s">
+        <v>522</v>
+      </c>
+      <c r="E487" t="s">
+        <v>522</v>
+      </c>
       <c r="F487" t="s">
         <v>1010</v>
+      </c>
+      <c r="G487" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I487" t="s">
+        <v>1342</v>
+      </c>
+      <c r="J487" t="s">
+        <v>1346</v>
       </c>
       <c r="K487" t="s">
         <v>1010</v>
@@ -19505,8 +19760,23 @@
       <c r="B488" t="s">
         <v>496</v>
       </c>
+      <c r="D488" t="s">
+        <v>522</v>
+      </c>
+      <c r="E488" t="s">
+        <v>522</v>
+      </c>
       <c r="F488" t="s">
         <v>1011</v>
+      </c>
+      <c r="G488" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I488" t="s">
+        <v>1342</v>
+      </c>
+      <c r="J488" t="s">
+        <v>1346</v>
       </c>
       <c r="K488" t="s">
         <v>1011</v>
@@ -19591,8 +19861,20 @@
       <c r="B492" t="s">
         <v>500</v>
       </c>
+      <c r="D492" t="s">
+        <v>523</v>
+      </c>
+      <c r="E492" t="s">
+        <v>523</v>
+      </c>
       <c r="F492" t="s">
         <v>1015</v>
+      </c>
+      <c r="I492" t="s">
+        <v>1343</v>
+      </c>
+      <c r="J492" t="s">
+        <v>1346</v>
       </c>
       <c r="K492" t="s">
         <v>1819</v>
@@ -19605,8 +19887,20 @@
       <c r="B493" t="s">
         <v>501</v>
       </c>
+      <c r="D493" t="s">
+        <v>523</v>
+      </c>
+      <c r="E493" t="s">
+        <v>523</v>
+      </c>
       <c r="F493" t="s">
         <v>1015</v>
+      </c>
+      <c r="I493" t="s">
+        <v>1343</v>
+      </c>
+      <c r="J493" t="s">
+        <v>1346</v>
       </c>
       <c r="K493" t="s">
         <v>1015</v>
@@ -19713,8 +20007,23 @@
       <c r="B499" t="s">
         <v>507</v>
       </c>
+      <c r="D499" t="s">
+        <v>522</v>
+      </c>
+      <c r="E499" t="s">
+        <v>522</v>
+      </c>
       <c r="F499" t="s">
         <v>1021</v>
+      </c>
+      <c r="G499" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I499" t="s">
+        <v>1344</v>
+      </c>
+      <c r="J499" t="s">
+        <v>1346</v>
       </c>
       <c r="K499" t="s">
         <v>1021</v>
@@ -19727,8 +20036,23 @@
       <c r="B500" t="s">
         <v>508</v>
       </c>
+      <c r="D500" t="s">
+        <v>522</v>
+      </c>
+      <c r="E500" t="s">
+        <v>522</v>
+      </c>
       <c r="F500" t="s">
         <v>1022</v>
+      </c>
+      <c r="G500" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I500" t="s">
+        <v>1344</v>
+      </c>
+      <c r="J500" t="s">
+        <v>1346</v>
       </c>
       <c r="K500" t="s">
         <v>1022</v>

</xml_diff>

<commit_message>
changed uploaded files to be moved to prior folder instead of copied
</commit_message>
<xml_diff>
--- a/UpdatedFiles/CSProvisioning.xlsx
+++ b/UpdatedFiles/CSProvisioning.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="1835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4078" uniqueCount="1835">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -11246,6 +11246,9 @@
       <c r="G185" t="s">
         <v>1045</v>
       </c>
+      <c r="I185" t="s">
+        <v>1160</v>
+      </c>
       <c r="J185" t="s">
         <v>1347</v>
       </c>
@@ -11272,6 +11275,9 @@
       <c r="G186" t="s">
         <v>1036</v>
       </c>
+      <c r="I186" t="s">
+        <v>1160</v>
+      </c>
       <c r="J186" t="s">
         <v>1347</v>
       </c>
@@ -11298,6 +11304,9 @@
       <c r="G187" t="s">
         <v>1042</v>
       </c>
+      <c r="I187" t="s">
+        <v>1160</v>
+      </c>
       <c r="J187" t="s">
         <v>1347</v>
       </c>
@@ -11324,6 +11333,9 @@
       <c r="G188" t="s">
         <v>1042</v>
       </c>
+      <c r="I188" t="s">
+        <v>1160</v>
+      </c>
       <c r="J188" t="s">
         <v>1347</v>
       </c>
@@ -11350,6 +11362,9 @@
       <c r="G189" t="s">
         <v>1036</v>
       </c>
+      <c r="I189" t="s">
+        <v>1160</v>
+      </c>
       <c r="J189" t="s">
         <v>1347</v>
       </c>
@@ -11376,6 +11391,9 @@
       <c r="G190" t="s">
         <v>1036</v>
       </c>
+      <c r="I190" t="s">
+        <v>1160</v>
+      </c>
       <c r="J190" t="s">
         <v>1347</v>
       </c>
@@ -11402,6 +11420,9 @@
       <c r="G191" t="s">
         <v>1036</v>
       </c>
+      <c r="I191" t="s">
+        <v>1160</v>
+      </c>
       <c r="J191" t="s">
         <v>1347</v>
       </c>
@@ -11428,6 +11449,9 @@
       <c r="G192" t="s">
         <v>1036</v>
       </c>
+      <c r="I192" t="s">
+        <v>1160</v>
+      </c>
       <c r="J192" t="s">
         <v>1347</v>
       </c>
@@ -11454,6 +11478,9 @@
       <c r="G193" t="s">
         <v>1036</v>
       </c>
+      <c r="I193" t="s">
+        <v>1160</v>
+      </c>
       <c r="J193" t="s">
         <v>1347</v>
       </c>
@@ -11480,6 +11507,9 @@
       <c r="G194" t="s">
         <v>1036</v>
       </c>
+      <c r="I194" t="s">
+        <v>1160</v>
+      </c>
       <c r="J194" t="s">
         <v>1347</v>
       </c>
@@ -19362,6 +19392,9 @@
       <c r="F466" t="s">
         <v>990</v>
       </c>
+      <c r="G466" t="s">
+        <v>1038</v>
+      </c>
       <c r="I466" t="s">
         <v>1340</v>
       </c>
@@ -19388,6 +19421,9 @@
       <c r="F467" t="s">
         <v>991</v>
       </c>
+      <c r="G467" t="s">
+        <v>1038</v>
+      </c>
       <c r="I467" t="s">
         <v>1340</v>
       </c>
@@ -19414,6 +19450,9 @@
       <c r="F468" t="s">
         <v>992</v>
       </c>
+      <c r="G468" t="s">
+        <v>1038</v>
+      </c>
       <c r="I468" t="s">
         <v>1340</v>
       </c>
@@ -19440,6 +19479,9 @@
       <c r="F469" t="s">
         <v>993</v>
       </c>
+      <c r="G469" t="s">
+        <v>1038</v>
+      </c>
       <c r="I469" t="s">
         <v>1340</v>
       </c>
@@ -19466,6 +19508,9 @@
       <c r="F470" t="s">
         <v>994</v>
       </c>
+      <c r="G470" t="s">
+        <v>1038</v>
+      </c>
       <c r="I470" t="s">
         <v>1340</v>
       </c>
@@ -19492,6 +19537,9 @@
       <c r="F471" t="s">
         <v>994</v>
       </c>
+      <c r="G471" t="s">
+        <v>1038</v>
+      </c>
       <c r="I471" t="s">
         <v>1340</v>
       </c>
@@ -19518,6 +19566,12 @@
       <c r="F472" t="s">
         <v>995</v>
       </c>
+      <c r="G472" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I472" t="s">
+        <v>1341</v>
+      </c>
       <c r="J472" t="s">
         <v>1346</v>
       </c>
@@ -19541,6 +19595,12 @@
       <c r="F473" t="s">
         <v>996</v>
       </c>
+      <c r="G473" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I473" t="s">
+        <v>1341</v>
+      </c>
       <c r="J473" t="s">
         <v>1346</v>
       </c>
@@ -19564,6 +19624,12 @@
       <c r="F474" t="s">
         <v>997</v>
       </c>
+      <c r="G474" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I474" t="s">
+        <v>1341</v>
+      </c>
       <c r="J474" t="s">
         <v>1346</v>
       </c>
@@ -19587,6 +19653,12 @@
       <c r="F475" t="s">
         <v>998</v>
       </c>
+      <c r="G475" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I475" t="s">
+        <v>1341</v>
+      </c>
       <c r="J475" t="s">
         <v>1346</v>
       </c>
@@ -19610,6 +19682,12 @@
       <c r="F476" t="s">
         <v>999</v>
       </c>
+      <c r="G476" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I476" t="s">
+        <v>1341</v>
+      </c>
       <c r="J476" t="s">
         <v>1346</v>
       </c>
@@ -19633,6 +19711,12 @@
       <c r="F477" t="s">
         <v>1000</v>
       </c>
+      <c r="G477" t="s">
+        <v>1038</v>
+      </c>
+      <c r="I477" t="s">
+        <v>1341</v>
+      </c>
       <c r="J477" t="s">
         <v>1346</v>
       </c>
@@ -20033,6 +20117,9 @@
       <c r="F491" t="s">
         <v>1014</v>
       </c>
+      <c r="G491" t="s">
+        <v>1039</v>
+      </c>
       <c r="I491" t="s">
         <v>1343</v>
       </c>
@@ -20059,6 +20146,9 @@
       <c r="F492" t="s">
         <v>1015</v>
       </c>
+      <c r="G492" t="s">
+        <v>1039</v>
+      </c>
       <c r="I492" t="s">
         <v>1343</v>
       </c>
@@ -20085,6 +20175,9 @@
       <c r="F493" t="s">
         <v>1015</v>
       </c>
+      <c r="G493" t="s">
+        <v>1039</v>
+      </c>
       <c r="I493" t="s">
         <v>1343</v>
       </c>
@@ -20110,6 +20203,9 @@
       </c>
       <c r="F494" t="s">
         <v>1016</v>
+      </c>
+      <c r="G494" t="s">
+        <v>1039</v>
       </c>
       <c r="I494" t="s">
         <v>1343</v>

</xml_diff>